<commit_message>
checkpoint g13; feito g13.7
</commit_message>
<xml_diff>
--- a/Data/g13.7.xlsx
+++ b/Data/g13.7.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -387,16 +463,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>25.6</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>28.8</v>
       </c>
     </row>
     <row r="3">
@@ -407,16 +483,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>23.8</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>30.4</v>
       </c>
     </row>
     <row r="4">
@@ -427,7 +503,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -435,8 +511,8 @@
           <t>01/07/2019</t>
         </is>
       </c>
-      <c r="D4">
-        <v>13.4</v>
+      <c r="D4" t="n">
+        <v>29.8</v>
       </c>
     </row>
     <row r="5">
@@ -452,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>29.8</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>27.4</v>
       </c>
     </row>
     <row r="6">
@@ -467,16 +543,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>3.8</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>27.7</v>
       </c>
     </row>
     <row r="7">
@@ -487,16 +563,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>3.5</v>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>28.1</v>
       </c>
     </row>
     <row r="8">
@@ -507,16 +583,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>27.4</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>27.9</v>
       </c>
     </row>
     <row r="9">
@@ -527,16 +603,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>24.3</v>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -547,16 +623,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>13.8</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>29.1</v>
       </c>
     </row>
     <row r="11">
@@ -572,11 +648,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>27.4</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>28.6</v>
       </c>
     </row>
     <row r="12">
@@ -587,16 +663,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>4.2</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>28.3</v>
       </c>
     </row>
     <row r="13">
@@ -607,16 +683,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>2.9</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>29.5</v>
       </c>
     </row>
     <row r="14">
@@ -627,16 +703,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>28.8</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>27.1</v>
       </c>
     </row>
     <row r="15">
@@ -647,16 +723,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>23.3</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="16">
@@ -667,16 +743,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D16">
-        <v>13.2</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row r="17">
@@ -692,11 +768,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D17">
-        <v>27.7</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>23.4</v>
       </c>
     </row>
     <row r="18">
@@ -707,16 +783,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D18">
-        <v>4.6</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>22.7</v>
       </c>
     </row>
     <row r="19">
@@ -727,16 +803,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D19">
-        <v>2.5</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>24.9</v>
       </c>
     </row>
     <row r="20">
@@ -747,16 +823,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D20">
-        <v>28.2</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>25.5</v>
       </c>
     </row>
     <row r="21">
@@ -767,16 +843,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D21">
-        <v>21</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>24.4</v>
       </c>
     </row>
     <row r="22">
@@ -787,16 +863,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D22">
-        <v>15.9</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>24.6</v>
       </c>
     </row>
     <row r="23">
@@ -812,11 +888,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D23">
-        <v>28.1</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>24.2</v>
       </c>
     </row>
     <row r="24">
@@ -827,16 +903,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D24">
-        <v>4.6</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>24.4</v>
       </c>
     </row>
     <row r="25">
@@ -847,16 +923,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Conta própria</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D25">
-        <v>2.1</v>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>23.9</v>
       </c>
     </row>
     <row r="26">
@@ -867,16 +943,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D26">
-        <v>28.6</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3.9</v>
       </c>
     </row>
     <row r="27">
@@ -887,16 +963,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D27">
-        <v>21.1</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.4</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +983,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D28">
-        <v>15.2</v>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>3.8</v>
       </c>
     </row>
     <row r="29">
@@ -927,16 +1003,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D29">
-        <v>27.9</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4.2</v>
       </c>
     </row>
     <row r="30">
@@ -952,11 +1028,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D30">
-        <v>4.1</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4.6</v>
       </c>
     </row>
     <row r="31">
@@ -967,16 +1043,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D31">
-        <v>3.1</v>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>4.6</v>
       </c>
     </row>
     <row r="32">
@@ -987,16 +1063,16 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
-      </c>
-      <c r="D32">
-        <v>25.2</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>4.1</v>
       </c>
     </row>
     <row r="33">
@@ -1007,7 +1083,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1015,8 +1091,8 @@
           <t>01/10/2020</t>
         </is>
       </c>
-      <c r="D33">
-        <v>22.1</v>
+      <c r="D33" t="n">
+        <v>4.9</v>
       </c>
     </row>
     <row r="34">
@@ -1027,16 +1103,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
-      </c>
-      <c r="D34">
-        <v>14.3</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>3.1</v>
       </c>
     </row>
     <row r="35">
@@ -1047,16 +1123,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
-      </c>
-      <c r="D35">
-        <v>30</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="36">
@@ -1072,11 +1148,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
-      </c>
-      <c r="D36">
-        <v>4.9</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>4.4</v>
       </c>
     </row>
     <row r="37">
@@ -1087,16 +1163,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
-      </c>
-      <c r="D37">
-        <v>3.5</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>4.8</v>
       </c>
     </row>
     <row r="38">
@@ -1107,16 +1183,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D38">
-        <v>27</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1127,16 +1203,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D39">
-        <v>22.6</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>5.8</v>
       </c>
     </row>
     <row r="40">
@@ -1147,16 +1223,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D40">
-        <v>14.9</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>4.9</v>
       </c>
     </row>
     <row r="41">
@@ -1167,16 +1243,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D41">
-        <v>29.1</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="42">
@@ -1192,11 +1268,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D42">
-        <v>3.1</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -1207,16 +1283,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D43">
-        <v>3.2</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>4.1</v>
       </c>
     </row>
     <row r="44">
@@ -1227,16 +1303,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D44">
-        <v>25.3</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>4.2</v>
       </c>
     </row>
     <row r="45">
@@ -1247,16 +1323,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D45">
-        <v>22.7</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="46">
@@ -1267,16 +1343,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D46">
-        <v>16.9</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="47">
@@ -1287,16 +1363,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D47">
-        <v>28.6</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -1312,11 +1388,11 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D48">
-        <v>3.2</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>4.5</v>
       </c>
     </row>
     <row r="49">
@@ -1327,16 +1403,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Empregador</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D49">
-        <v>3.3</v>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>4.6</v>
       </c>
     </row>
     <row r="50">
@@ -1352,11 +1428,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D50">
-        <v>23.7</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>27.3</v>
       </c>
     </row>
     <row r="51">
@@ -1367,16 +1443,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D51">
-        <v>24.7</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="52">
@@ -1387,16 +1463,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D52">
-        <v>16</v>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>25.6</v>
       </c>
     </row>
     <row r="53">
@@ -1407,16 +1483,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D53">
-        <v>28.3</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>27.4</v>
       </c>
     </row>
     <row r="54">
@@ -1427,16 +1503,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D54">
-        <v>4.4</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>28.8</v>
       </c>
     </row>
     <row r="55">
@@ -1447,16 +1523,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>3</v>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>28.2</v>
       </c>
     </row>
     <row r="56">
@@ -1472,11 +1548,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
-      <c r="D56">
-        <v>25</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>28.6</v>
       </c>
     </row>
     <row r="57">
@@ -1487,16 +1563,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
-      <c r="D57">
-        <v>22.6</v>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>25.2</v>
       </c>
     </row>
     <row r="58">
@@ -1507,16 +1583,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
-      <c r="D58">
-        <v>14.5</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="59">
@@ -1527,16 +1603,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
-      <c r="D59">
-        <v>29.5</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>25.3</v>
       </c>
     </row>
     <row r="60">
@@ -1547,16 +1623,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
-      <c r="D60">
-        <v>4.8</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>23.7</v>
       </c>
     </row>
     <row r="61">
@@ -1567,7 +1643,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1575,8 +1651,8 @@
           <t>01/10/2021</t>
         </is>
       </c>
-      <c r="D61">
-        <v>3.6</v>
+      <c r="D61" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="62">
@@ -1595,7 +1671,7 @@
           <t>01/01/2022</t>
         </is>
       </c>
-      <c r="D62">
+      <c r="D62" t="n">
         <v>26.4</v>
       </c>
     </row>
@@ -1607,16 +1683,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D63">
-        <v>24.8</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="64">
@@ -1627,16 +1703,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D64">
-        <v>13.7</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>27.3</v>
       </c>
     </row>
     <row r="65">
@@ -1647,16 +1723,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D65">
-        <v>27.1</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>28.7</v>
       </c>
     </row>
     <row r="66">
@@ -1667,16 +1743,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D66">
-        <v>5</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>28.6</v>
       </c>
     </row>
     <row r="67">
@@ -1687,16 +1763,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D67">
-        <v>3</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>28.2</v>
       </c>
     </row>
     <row r="68">
@@ -1712,11 +1788,11 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D68">
-        <v>27</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>27.1</v>
       </c>
     </row>
     <row r="69">
@@ -1727,16 +1803,16 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D69">
-        <v>24.8</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>28.2</v>
       </c>
     </row>
     <row r="70">
@@ -1747,16 +1823,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D70">
-        <v>13.4</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>29.3</v>
       </c>
     </row>
     <row r="71">
@@ -1767,16 +1843,16 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D71">
-        <v>26</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>30.2</v>
       </c>
     </row>
     <row r="72">
@@ -1787,16 +1863,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D72">
-        <v>5.8</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="73">
@@ -1807,16 +1883,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado com carteira</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D73">
-        <v>3</v>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>30.3</v>
       </c>
     </row>
     <row r="74">
@@ -1827,16 +1903,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D74">
-        <v>27.3</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>22.2</v>
       </c>
     </row>
     <row r="75">
@@ -1852,11 +1928,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D75">
-        <v>23.7</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>21.8</v>
       </c>
     </row>
     <row r="76">
@@ -1867,16 +1943,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D76">
-        <v>15.2</v>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>23.8</v>
       </c>
     </row>
     <row r="77">
@@ -1887,16 +1963,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D77">
-        <v>25.8</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>24.3</v>
       </c>
     </row>
     <row r="78">
@@ -1907,16 +1983,16 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D78">
-        <v>4.9</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>23.3</v>
       </c>
     </row>
     <row r="79">
@@ -1927,16 +2003,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D79">
-        <v>3.2</v>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="80">
@@ -1947,16 +2023,16 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D80">
-        <v>28.7</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>21.1</v>
       </c>
     </row>
     <row r="81">
@@ -1972,11 +2048,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D81">
-        <v>24.7</v>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>22.1</v>
       </c>
     </row>
     <row r="82">
@@ -1987,16 +2063,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D82">
-        <v>15.5</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>22.6</v>
       </c>
     </row>
     <row r="83">
@@ -2007,16 +2083,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D83">
-        <v>23.4</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>22.7</v>
       </c>
     </row>
     <row r="84">
@@ -2027,16 +2103,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D84">
-        <v>4.3</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>24.7</v>
       </c>
     </row>
     <row r="85">
@@ -2047,16 +2123,16 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D85">
-        <v>3.4</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>22.6</v>
       </c>
     </row>
     <row r="86">
@@ -2067,16 +2143,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D86">
-        <v>28.6</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>24.8</v>
       </c>
     </row>
     <row r="87">
@@ -2092,11 +2168,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D87">
-        <v>25.7</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>24.8</v>
       </c>
     </row>
     <row r="88">
@@ -2107,16 +2183,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D88">
-        <v>15.7</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>23.7</v>
       </c>
     </row>
     <row r="89">
@@ -2127,16 +2203,16 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D89">
-        <v>22.7</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>24.7</v>
       </c>
     </row>
     <row r="90">
@@ -2147,7 +2223,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2155,8 +2231,8 @@
           <t>01/01/2023</t>
         </is>
       </c>
-      <c r="D90">
-        <v>4</v>
+      <c r="D90" t="n">
+        <v>25.7</v>
       </c>
     </row>
     <row r="91">
@@ -2167,16 +2243,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D91">
-        <v>3.2</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>24.2</v>
       </c>
     </row>
     <row r="92">
@@ -2187,16 +2263,16 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D92">
-        <v>28.2</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>24.6</v>
       </c>
     </row>
     <row r="93">
@@ -2212,11 +2288,11 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D93">
-        <v>24.2</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>25.4</v>
       </c>
     </row>
     <row r="94">
@@ -2227,16 +2303,16 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D94">
-        <v>15.6</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>24.3</v>
       </c>
     </row>
     <row r="95">
@@ -2247,16 +2323,16 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D95">
-        <v>24.9</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>23.4</v>
       </c>
     </row>
     <row r="96">
@@ -2267,16 +2343,16 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D96">
-        <v>4.1</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>23.8</v>
       </c>
     </row>
     <row r="97">
@@ -2287,16 +2363,16 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor privado sem carteira</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D97">
-        <v>2.9</v>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>23.5</v>
       </c>
     </row>
     <row r="98">
@@ -2307,16 +2383,16 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D98">
-        <v>27.1</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="99">
@@ -2327,16 +2403,16 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D99">
-        <v>24.6</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="100">
@@ -2352,11 +2428,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D100">
-        <v>15.4</v>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>13.4</v>
       </c>
     </row>
     <row r="101">
@@ -2367,16 +2443,16 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D101">
-        <v>25.5</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>13.8</v>
       </c>
     </row>
     <row r="102">
@@ -2387,16 +2463,16 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D102">
-        <v>4.2</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>13.2</v>
       </c>
     </row>
     <row r="103">
@@ -2407,16 +2483,16 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D103">
-        <v>3.2</v>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>15.9</v>
       </c>
     </row>
     <row r="104">
@@ -2427,16 +2503,16 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D104">
-        <v>28.2</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>15.2</v>
       </c>
     </row>
     <row r="105">
@@ -2447,16 +2523,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D105">
-        <v>25.4</v>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>14.3</v>
       </c>
     </row>
     <row r="106">
@@ -2472,11 +2548,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D106">
-        <v>15.7</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>14.9</v>
       </c>
     </row>
     <row r="107">
@@ -2487,16 +2563,16 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D107">
-        <v>24.4</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>16.9</v>
       </c>
     </row>
     <row r="108">
@@ -2507,16 +2583,16 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D108">
-        <v>3.5</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="109">
@@ -2527,16 +2603,16 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D109">
-        <v>2.8</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>14.5</v>
       </c>
     </row>
     <row r="110">
@@ -2547,16 +2623,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D110">
-        <v>29.3</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>13.7</v>
       </c>
     </row>
     <row r="111">
@@ -2567,16 +2643,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D111">
-        <v>24.3</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>13.4</v>
       </c>
     </row>
     <row r="112">
@@ -2592,10 +2668,10 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D112">
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
         <v>15.2</v>
       </c>
     </row>
@@ -2607,16 +2683,16 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D113">
-        <v>24.6</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>15.5</v>
       </c>
     </row>
     <row r="114">
@@ -2627,16 +2703,16 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D114">
-        <v>3.6</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>15.7</v>
       </c>
     </row>
     <row r="115">
@@ -2647,16 +2723,16 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D115">
-        <v>3</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>15.6</v>
       </c>
     </row>
     <row r="116">
@@ -2667,16 +2743,16 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D116">
-        <v>30.2</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>15.4</v>
       </c>
     </row>
     <row r="117">
@@ -2687,16 +2763,16 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D117">
-        <v>23.4</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>15.7</v>
       </c>
     </row>
     <row r="118">
@@ -2712,11 +2788,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D118">
-        <v>15.3</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>15.2</v>
       </c>
     </row>
     <row r="119">
@@ -2727,7 +2803,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2735,8 +2811,8 @@
           <t>01/04/2024</t>
         </is>
       </c>
-      <c r="D119">
-        <v>24.2</v>
+      <c r="D119" t="n">
+        <v>15.3</v>
       </c>
     </row>
     <row r="120">
@@ -2747,16 +2823,16 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D120">
-        <v>4</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>14.7</v>
       </c>
     </row>
     <row r="121">
@@ -2767,16 +2843,16 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Trabalhador familiar auxiliar</t>
+          <t>Setor público</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D121">
-        <v>2.7</v>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>15.3</v>
       </c>
     </row>
     <row r="122">
@@ -2787,16 +2863,16 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Setor privado com carteira</t>
+          <t>Trabalhador familiar auxiliar</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D122">
-        <v>30</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>3.8</v>
       </c>
     </row>
     <row r="123">
@@ -2807,16 +2883,16 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Setor privado sem carteira</t>
+          <t>Trabalhador familiar auxiliar</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D123">
-        <v>23.8</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="124">
@@ -2827,16 +2903,16 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Setor público</t>
+          <t>Trabalhador familiar auxiliar</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D124">
-        <v>14.7</v>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="125">
@@ -2847,16 +2923,16 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Conta própria</t>
+          <t>Trabalhador familiar auxiliar</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D125">
-        <v>24.4</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>2.9</v>
       </c>
     </row>
     <row r="126">
@@ -2867,16 +2943,16 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Empregador</t>
+          <t>Trabalhador familiar auxiliar</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D126">
-        <v>4.5</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="127">
@@ -2892,14 +2968,374 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D127">
+      <c r="D144" t="n">
         <v>2.6</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Trabalhador familiar auxiliar</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>